<commit_message>
Update 6 for GUI Reorganization
</commit_message>
<xml_diff>
--- a/testCustomFile/BalloonData_1obj.xlsx
+++ b/testCustomFile/BalloonData_1obj.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{44F63096-3D45-4789-B1C1-717D2B33264A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{2E0B384F-50F2-4DD8-B093-089C4CD4DEF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <t>BalloonName</t>
   </si>
   <si>
-    <t>LaunchTime</t>
+    <t>LaunchTime (STK format)</t>
   </si>
   <si>
     <t>LaunchLat</t>
@@ -399,11 +399,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EA77EED-E8BD-4E37-B2D0-B55496EC4D81}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B004B272-2E6A-4D2B-BDBB-1078DA9742C1}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -439,13 +439,13 @@
         <v>35</v>
       </c>
       <c r="D2">
-        <v>-82</v>
+        <v>-80</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>